<commit_message>
adicionando excel com normalização 2
</commit_message>
<xml_diff>
--- a/Morganum/normalizacao.xlsx
+++ b/Morganum/normalizacao.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7136c66459876bfe/01_Garoto_de_Programa/02_Materias_Faculdade/sem3_trabalho_final/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7136c66459876bfe/01_Garoto_de_Programa/02_Materias_Faculdade/sem3_trabalho_final/FataMorgana/Morganum/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="40" documentId="8_{BB408C17-E3B0-4172-A77C-F1887326046B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ABD4B1A4-BC98-47F6-9D55-3A4F92A1DC9D}"/>
+  <xr:revisionPtr revIDLastSave="119" documentId="8_{BB408C17-E3B0-4172-A77C-F1887326046B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B796B13A-D041-47A0-8573-CF4E1F26DD86}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F93F0CA4-3D93-4B95-B704-105B3F7897BF}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="74">
   <si>
     <t>cliente</t>
   </si>
@@ -71,9 +71,6 @@
     <t>funcionario</t>
   </si>
   <si>
-    <t>matricula</t>
-  </si>
-  <si>
     <t>cargo</t>
   </si>
   <si>
@@ -95,9 +92,6 @@
     <t>user</t>
   </si>
   <si>
-    <t>mog</t>
-  </si>
-  <si>
     <t>dt_ult_acss</t>
   </si>
   <si>
@@ -131,9 +125,6 @@
     <t>cidade</t>
   </si>
   <si>
-    <t>address</t>
-  </si>
-  <si>
     <t>bairro</t>
   </si>
   <si>
@@ -150,6 +141,123 @@
   </si>
   <si>
     <t>referencia</t>
+  </si>
+  <si>
+    <t>livro</t>
+  </si>
+  <si>
+    <t>titulo</t>
+  </si>
+  <si>
+    <t>autor</t>
+  </si>
+  <si>
+    <t>gen_lit</t>
+  </si>
+  <si>
+    <t>editora</t>
+  </si>
+  <si>
+    <t>edicao</t>
+  </si>
+  <si>
+    <t>impressao</t>
+  </si>
+  <si>
+    <t>idioma</t>
+  </si>
+  <si>
+    <t>data_publi</t>
+  </si>
+  <si>
+    <t>descricao</t>
+  </si>
+  <si>
+    <t>num_pagina</t>
+  </si>
+  <si>
+    <t>isbn_13</t>
+  </si>
+  <si>
+    <t>isbn_10</t>
+  </si>
+  <si>
+    <t>pedido</t>
+  </si>
+  <si>
+    <t>id_ped</t>
+  </si>
+  <si>
+    <t>data_ped</t>
+  </si>
+  <si>
+    <t>hr_ped</t>
+  </si>
+  <si>
+    <t>mtd_envio</t>
+  </si>
+  <si>
+    <t>mtd_pag</t>
+  </si>
+  <si>
+    <t>coment</t>
+  </si>
+  <si>
+    <t>itens_pedido</t>
+  </si>
+  <si>
+    <t>total_ped</t>
+  </si>
+  <si>
+    <t>id_item</t>
+  </si>
+  <si>
+    <t>qnt_item</t>
+  </si>
+  <si>
+    <t>qnt_livro</t>
+  </si>
+  <si>
+    <t>preco_livro</t>
+  </si>
+  <si>
+    <t>desconto</t>
+  </si>
+  <si>
+    <t>id_func</t>
+  </si>
+  <si>
+    <t>morgs_cliente</t>
+  </si>
+  <si>
+    <t>id_morg</t>
+  </si>
+  <si>
+    <t>pontos</t>
+  </si>
+  <si>
+    <t>data_acumulo</t>
+  </si>
+  <si>
+    <t>status_ped</t>
+  </si>
+  <si>
+    <t>status_morg</t>
+  </si>
+  <si>
+    <t>comm_func</t>
+  </si>
+  <si>
+    <t>id_comm</t>
+  </si>
+  <si>
+    <t>valor_comm</t>
+  </si>
+  <si>
+    <t>data_pag</t>
+  </si>
+  <si>
+    <t>logradouro</t>
   </si>
 </sst>
 </file>
@@ -225,7 +333,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -233,6 +341,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -248,6 +357,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -567,10 +680,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69609D9A-472B-43C9-8BD6-7DD7F95D8EF4}">
-  <dimension ref="B3:E17"/>
+  <dimension ref="B3:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -581,12 +694,16 @@
     <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>0</v>
@@ -597,141 +714,273 @@
       <c r="E3" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="G3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>11</v>
+        <v>62</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>8</v>
+      <c r="C9" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="D9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="D11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="E12" s="3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="3" t="s">
+      <c r="G12" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="E13" s="3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D11" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E11" s="3" t="s">
+      <c r="G13" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="E14" s="3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E12" s="3" t="s">
+      <c r="G14" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="E15" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="E16" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E13" s="3" t="s">
+      <c r="G16" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E17" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E14" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E15" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E16" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E17" s="2" t="s">
-        <v>36</v>
+      <c r="G17" s="3" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adicionando script sql e iniciando CRUD
</commit_message>
<xml_diff>
--- a/Morganum/normalizacao.xlsx
+++ b/Morganum/normalizacao.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7136c66459876bfe/01_Garoto_de_Programa/02_Materias_Faculdade/sem3_trabalho_final/FataMorgana/Morganum/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="119" documentId="8_{BB408C17-E3B0-4172-A77C-F1887326046B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B796B13A-D041-47A0-8573-CF4E1F26DD86}"/>
+  <xr:revisionPtr revIDLastSave="126" documentId="8_{BB408C17-E3B0-4172-A77C-F1887326046B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{120903EC-64E1-463D-A821-47D8BAB0D30D}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F93F0CA4-3D93-4B95-B704-105B3F7897BF}"/>
+    <workbookView xWindow="-28920" yWindow="4050" windowWidth="29040" windowHeight="15720" xr2:uid="{F93F0CA4-3D93-4B95-B704-105B3F7897BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="74">
   <si>
     <t>cliente</t>
   </si>
@@ -293,7 +293,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -329,6 +329,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -341,7 +354,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -683,14 +696,13 @@
   <dimension ref="B3:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
@@ -734,12 +746,8 @@
       <c r="B4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>62</v>
-      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
         <v>21</v>
       </c>
@@ -789,11 +797,11 @@
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>18</v>
+      <c r="C6" s="7" t="s">
+        <v>33</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>12</v>
@@ -818,11 +826,8 @@
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="3" t="s">
         <v>4</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>19</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>15</v>
@@ -833,7 +838,7 @@
       <c r="G7" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="I7" s="3" t="s">
         <v>56</v>
       </c>
       <c r="J7" s="2" t="s">
@@ -847,11 +852,8 @@
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>8</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>16</v>
@@ -876,11 +878,8 @@
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>13</v>
@@ -916,6 +915,9 @@
       </c>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B11" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="D11" s="2" t="s">
         <v>33</v>
       </c>
@@ -925,11 +927,14 @@
       <c r="G11" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="I11" s="7" t="s">
+      <c r="I11" s="3" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B12" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="E12" s="3" t="s">
         <v>29</v>
       </c>
@@ -941,6 +946,9 @@
       </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="E13" s="3" t="s">
         <v>30</v>
       </c>

</xml_diff>